<commit_message>
modified code and updated dependencies
</commit_message>
<xml_diff>
--- a/TestResources/TestData.xlsx
+++ b/TestResources/TestData.xlsx
@@ -1,118 +1,141 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keshavmac/IdeaProjects/RestAssuredDemo/TestResources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CADDC5-CA84-0640-B64B-40F26448E9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Job</t>
-  </si>
-  <si>
-    <t>Peeyush</t>
-  </si>
-  <si>
-    <t>Engineer</t>
-  </si>
-  <si>
-    <t>Sudhir</t>
-  </si>
-  <si>
-    <t>Doctor</t>
-  </si>
-  <si>
-    <t>Manish</t>
-  </si>
-  <si>
-    <t>Lecturer</t>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Ravi shukla</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>ravishukla@gmail.com</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Prachi gupta</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>prachigupta@gmail.com</t>
+  </si>
+  <si>
+    <t>Gauri</t>
+  </si>
+  <si>
+    <t>gauri@gmail.com</t>
+  </si>
+  <si>
+    <t>Rachit</t>
+  </si>
+  <si>
+    <t>rachit@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
-    <font/>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="1">
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -302,52 +325,102 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911ABC88-F0A3-2F4E-B46E-8CE87D956C5B}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{761CD256-678E-5042-BAEF-BCA791D6829A}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{303644F5-2917-FD43-8A3C-C8898B25476E}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{EF6F7E0B-675B-764D-8FD0-7A1D51EF0689}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{DF635C6F-2BD4-4A46-9F35-D23C827A9CB4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>